<commit_message>
Results to excel and update torch
</commit_message>
<xml_diff>
--- a/logs/results.xlsx
+++ b/logs/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t xml:space="preserve">Accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time training</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time test</t>
   </si>
 </sst>
 </file>
@@ -182,10 +188,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
+      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -260,6 +266,12 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Option to do test after training and save results
</commit_message>
<xml_diff>
--- a/logs/results.xlsx
+++ b/logs/results.xlsx
@@ -13,7 +13,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -94,6 +94,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -114,6 +115,7 @@
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -191,14 +193,14 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.52"/>
@@ -211,7 +213,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="19" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -278,8 +280,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>